<commit_message>
Added batch get symbols
</commit_message>
<xml_diff>
--- a/Tickers.xlsx
+++ b/Tickers.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/286054357d240948/Github/Intro to Finance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D94F4875-31FF-40FD-95CD-E8385797BA8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="8_{D94F4875-31FF-40FD-95CD-E8385797BA8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E21145A4-FEA9-4301-A5DB-CBB6EB7D1080}"/>
   <bookViews>
-    <workbookView xWindow="-26355" yWindow="2775" windowWidth="24000" windowHeight="12855" xr2:uid="{AEDDC109-3F26-41B1-AD44-8411DA0AE54E}"/>
+    <workbookView xWindow="1290" yWindow="2970" windowWidth="21600" windowHeight="11835" xr2:uid="{AEDDC109-3F26-41B1-AD44-8411DA0AE54E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Commodity" sheetId="1" r:id="rId1"/>
-    <sheet name="XRef" sheetId="2" r:id="rId2"/>
+    <sheet name="Tickers" sheetId="3" r:id="rId1"/>
+    <sheet name="Commodity" sheetId="1" r:id="rId2"/>
+    <sheet name="XRef" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="54">
   <si>
     <t>Mth#</t>
   </si>
@@ -148,6 +149,57 @@
   </si>
   <si>
     <t>YrAdj</t>
+  </si>
+  <si>
+    <t>Crude</t>
+  </si>
+  <si>
+    <t>NatGas</t>
+  </si>
+  <si>
+    <t>NG</t>
+  </si>
+  <si>
+    <t>CRUDE</t>
+  </si>
+  <si>
+    <t>Ticker</t>
+  </si>
+  <si>
+    <t>CLF24.NYM</t>
+  </si>
+  <si>
+    <t>CLG23.NYM</t>
+  </si>
+  <si>
+    <t>CLH23.NYM</t>
+  </si>
+  <si>
+    <t>CLJ23.NYM</t>
+  </si>
+  <si>
+    <t>CLK23.NYM</t>
+  </si>
+  <si>
+    <t>CLM23.NYM</t>
+  </si>
+  <si>
+    <t>CLN23.NYM</t>
+  </si>
+  <si>
+    <t>CLQ23.NYM</t>
+  </si>
+  <si>
+    <t>CLU23.NYM</t>
+  </si>
+  <si>
+    <t>CLV23.NYM</t>
+  </si>
+  <si>
+    <t>CLX23.NYM</t>
+  </si>
+  <si>
+    <t>CLZ23.NYM</t>
   </si>
 </sst>
 </file>
@@ -156,7 +208,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -247,7 +299,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -275,6 +327,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -566,131 +622,89 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9818F960-3920-4012-8CC5-8A831A5672A3}">
-  <dimension ref="B2:C18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A4BE4C2-AD60-499F-9A7B-C4A7CE82571B}">
+  <dimension ref="A1:A13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="3" width="5" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="11.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B4" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" s="7">
-        <f ca="1">YEAR(NOW())</f>
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B5" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" s="7">
-        <f ca="1">MONTH(NOW())</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B7" s="2" t="str">
-        <f ca="1">$C$2&amp;XRef!D9&amp;RIGHT(XRef!F9,2)&amp;"."&amp;$C$3</f>
-        <v>CLF24.NYM</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B8" s="2" t="str">
-        <f ca="1">$C$2&amp;XRef!D10&amp;RIGHT(XRef!F10,2)&amp;"."&amp;$C$3</f>
-        <v>CLG23.NYM</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="2" t="str">
-        <f ca="1">$C$2&amp;XRef!D11&amp;RIGHT(XRef!F11,2)&amp;"."&amp;$C$3</f>
-        <v>CLH23.NYM</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="2" t="str">
-        <f ca="1">$C$2&amp;XRef!D12&amp;RIGHT(XRef!F12,2)&amp;"."&amp;$C$3</f>
-        <v>CLJ23.NYM</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="2" t="str">
-        <f ca="1">$C$2&amp;XRef!D13&amp;RIGHT(XRef!F13,2)&amp;"."&amp;$C$3</f>
-        <v>CLK23.NYM</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B12" s="2" t="str">
-        <f ca="1">$C$2&amp;XRef!D14&amp;RIGHT(XRef!F14,2)&amp;"."&amp;$C$3</f>
-        <v>CLM23.NYM</v>
-      </c>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="2" t="str">
-        <f ca="1">$C$2&amp;XRef!D15&amp;RIGHT(XRef!F15,2)&amp;"."&amp;$C$3</f>
-        <v>CLN23.NYM</v>
-      </c>
-    </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="2" t="str">
-        <f ca="1">$C$2&amp;XRef!D16&amp;RIGHT(XRef!F16,2)&amp;"."&amp;$C$3</f>
-        <v>CLQ23.NYM</v>
-      </c>
-    </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B15" s="2" t="str">
-        <f ca="1">$C$2&amp;XRef!D17&amp;RIGHT(XRef!F17,2)&amp;"."&amp;$C$3</f>
-        <v>CLU23.NYM</v>
-      </c>
-    </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="2" t="str">
-        <f ca="1">$C$2&amp;XRef!D18&amp;RIGHT(XRef!F18,2)&amp;"."&amp;$C$3</f>
-        <v>CLV23.NYM</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B17" s="2" t="str">
-        <f ca="1">$C$2&amp;XRef!D19&amp;RIGHT(XRef!F19,2)&amp;"."&amp;$C$3</f>
-        <v>CLX23.NYM</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B18" s="2" t="str">
-        <f ca="1">$C$2&amp;XRef!D20&amp;RIGHT(XRef!F20,2)&amp;"."&amp;$C$3</f>
-        <v>CLZ23.NYM</v>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -699,11 +713,162 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9818F960-3920-4012-8CC5-8A831A5672A3}">
+  <dimension ref="B2:D19"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7:C18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="2" max="2" width="6.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.28515625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="5" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="7">
+        <f ca="1">YEAR(NOW())</f>
+        <v>2023</v>
+      </c>
+      <c r="D4" s="7">
+        <f ca="1">YEAR(NOW())</f>
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="7">
+        <f ca="1">MONTH(NOW())</f>
+        <v>1</v>
+      </c>
+      <c r="D5" s="7">
+        <f ca="1">MONTH(NOW())</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="2" t="str">
+        <f ca="1">$C$2&amp;XRef!D9&amp;RIGHT(XRef!F9,2)&amp;"."&amp;$C$3</f>
+        <v>CLF24.NYM</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C8" s="2" t="str">
+        <f ca="1">$C$2&amp;XRef!D10&amp;RIGHT(XRef!F10,2)&amp;"."&amp;$C$3</f>
+        <v>CLG23.NYM</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C9" s="2" t="str">
+        <f ca="1">$C$2&amp;XRef!D11&amp;RIGHT(XRef!F11,2)&amp;"."&amp;$C$3</f>
+        <v>CLH23.NYM</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C10" s="2" t="str">
+        <f ca="1">$C$2&amp;XRef!D12&amp;RIGHT(XRef!F12,2)&amp;"."&amp;$C$3</f>
+        <v>CLJ23.NYM</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C11" s="2" t="str">
+        <f ca="1">$C$2&amp;XRef!D13&amp;RIGHT(XRef!F13,2)&amp;"."&amp;$C$3</f>
+        <v>CLK23.NYM</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C12" s="2" t="str">
+        <f ca="1">$C$2&amp;XRef!D14&amp;RIGHT(XRef!F14,2)&amp;"."&amp;$C$3</f>
+        <v>CLM23.NYM</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C13" s="2" t="str">
+        <f ca="1">$C$2&amp;XRef!D15&amp;RIGHT(XRef!F15,2)&amp;"."&amp;$C$3</f>
+        <v>CLN23.NYM</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C14" s="2" t="str">
+        <f ca="1">$C$2&amp;XRef!D16&amp;RIGHT(XRef!F16,2)&amp;"."&amp;$C$3</f>
+        <v>CLQ23.NYM</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C15" s="2" t="str">
+        <f ca="1">$C$2&amp;XRef!D17&amp;RIGHT(XRef!F17,2)&amp;"."&amp;$C$3</f>
+        <v>CLU23.NYM</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C16" s="2" t="str">
+        <f ca="1">$C$2&amp;XRef!D18&amp;RIGHT(XRef!F18,2)&amp;"."&amp;$C$3</f>
+        <v>CLV23.NYM</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C17" s="2" t="str">
+        <f ca="1">$C$2&amp;XRef!D19&amp;RIGHT(XRef!F19,2)&amp;"."&amp;$C$3</f>
+        <v>CLX23.NYM</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C18" s="2" t="str">
+        <f ca="1">$C$2&amp;XRef!D20&amp;RIGHT(XRef!F20,2)&amp;"."&amp;$C$3</f>
+        <v>CLZ23.NYM</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B19" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F21A8FDD-8A7F-4EC3-8A5E-DA299EE39273}">
   <dimension ref="B2:G20"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9:F20"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -722,7 +887,7 @@
       </c>
       <c r="D2" s="4">
         <f ca="1">NOW()</f>
-        <v>44943.494208217591</v>
+        <v>44945.65927650463</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.2">
@@ -741,6 +906,11 @@
       <c r="D4" s="2">
         <f ca="1">MONTH(D2)</f>
         <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B6" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Got rid of utilities 1 & 2. Replaced with keepers. Some bug fixes
</commit_message>
<xml_diff>
--- a/Tickers.xlsx
+++ b/Tickers.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="21" documentId="8_{D94F4875-31FF-40FD-95CD-E8385797BA8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E21145A4-FEA9-4301-A5DB-CBB6EB7D1080}"/>
   <bookViews>
-    <workbookView xWindow="1290" yWindow="2970" windowWidth="21600" windowHeight="11835" xr2:uid="{AEDDC109-3F26-41B1-AD44-8411DA0AE54E}"/>
+    <workbookView xWindow="-26955" yWindow="1185" windowWidth="21600" windowHeight="11835" xr2:uid="{AEDDC109-3F26-41B1-AD44-8411DA0AE54E}"/>
   </bookViews>
   <sheets>
     <sheet name="Tickers" sheetId="3" r:id="rId1"/>
@@ -633,7 +633,7 @@
   <dimension ref="A1:A13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection sqref="A1:A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -887,7 +887,7 @@
       </c>
       <c r="D2" s="4">
         <f ca="1">NOW()</f>
-        <v>44945.65927650463</v>
+        <v>44946.434097800928</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.2">

</xml_diff>